<commit_message>
Update App.jsx, styles.css, and package.json with new UI and dependencies
</commit_message>
<xml_diff>
--- a/public/спецпроекты.xlsx
+++ b/public/спецпроекты.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\telegram-mini-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62549C81-4A70-4AE7-81B5-6B1F568A1AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75508051-36D6-49EA-B652-E442705215CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Шеф сделал" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="576">
   <si>
     <t>Ссылка</t>
   </si>
@@ -1486,6 +1486,294 @@
   </si>
   <si>
     <t>07.07 - 13.07</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-222134246_4225</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13190</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23897</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157226882919841</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-47908301_2790049</t>
+  </si>
+  <si>
+    <t>https://ok.ru/raionklg/topic/157391860724697</t>
+  </si>
+  <si>
+    <t>https://ok.ru/goodnewsklg/topic/158024336233805</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-222134246_4229</t>
+  </si>
+  <si>
+    <t>https://t.me/klgzhest/46907</t>
+  </si>
+  <si>
+    <t>https://t.me/klgzhest/46898</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13208</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157229095218593</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23933</t>
+  </si>
+  <si>
+    <t>https://vk.com/clip-204895491_456240655</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23995</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157233231981985</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157234877197729</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_24017</t>
+  </si>
+  <si>
+    <t>https://vk.com/clip-204895491_456240654</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157232285904289</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23973</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23983</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13244</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157231869095329</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157232006065569</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23978</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13237</t>
+  </si>
+  <si>
+    <t>https://t.me/sdelanounas_ru/45377</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157231733632417</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13233</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23969</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157230687088033</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23956</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13225</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-47908301_2790764</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-222134246_4240</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000003608141/topic/158025978893645</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13217</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23943</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157230366092705</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-47908301_2790723</t>
+  </si>
+  <si>
+    <t>https://ok.ru/raionklg/topic/157393264374745</t>
+  </si>
+  <si>
+    <t>https://t.me/klgzhest/46934</t>
+  </si>
+  <si>
+    <t>https://t.me/klgmem365/857</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-224181694_3781</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-187624481_42216</t>
+  </si>
+  <si>
+    <t>https://ok.ru/kalugazanashih/topic/157393052824537</t>
+  </si>
+  <si>
+    <t>https://vk.com/clip-222134246_456239605</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-79894807_450928</t>
+  </si>
+  <si>
+    <t>https://ok.ru/goodnewsklg/topic/158025652524365</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-222134246_4237</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000003608141/topic/158022503912781</t>
+  </si>
+  <si>
+    <t>https://t.me/Srochno_ii_tochno/9659</t>
+  </si>
+  <si>
+    <t>https://t.me/Mosalskaya_telezhka/9941</t>
+  </si>
+  <si>
+    <t>https://t.me/ZHizdra_40/5703</t>
+  </si>
+  <si>
+    <t>https://t.me/Na_rajone_Duminichi/16170</t>
+  </si>
+  <si>
+    <t>https://t.me/Suharik_lajf/11391</t>
+  </si>
+  <si>
+    <t>https://t.me/Kirovv40/6398</t>
+  </si>
+  <si>
+    <t>https://t.me/V_Dzerzhinskom_raione/7648</t>
+  </si>
+  <si>
+    <t>https://t.me/kuibyshevskij_obozrevatel/2141</t>
+  </si>
+  <si>
+    <t>https://t.me/Medyn_korotko_o_glavnom/6010</t>
+  </si>
+  <si>
+    <t>https://t.me/Zdes_i_seichas_po_kozelski/12097</t>
+  </si>
+  <si>
+    <t>https://t.me/Ulyanovskij_perepoloh/3018</t>
+  </si>
+  <si>
+    <t>https://t.me/Babyninskij_informer/6197</t>
+  </si>
+  <si>
+    <t>https://t.me/Borovskaya_stengazeta/6115</t>
+  </si>
+  <si>
+    <t>https://t.me/Lyudinovskij_standart/7368</t>
+  </si>
+  <si>
+    <t>https://t.me/Yuhnov_Pro_nastoyashchee/8208</t>
+  </si>
+  <si>
+    <t>https://t.me/Privet_Baryatino/5732</t>
+  </si>
+  <si>
+    <t>https://t.me/Meshchovskie_kuranty/6373</t>
+  </si>
+  <si>
+    <t>https://t.me/Prosto_ZHukovskij_rajon/5583</t>
+  </si>
+  <si>
+    <t>https://t.me/Spas_novosti/8245</t>
+  </si>
+  <si>
+    <t>https://t.me/Tarusa_zdes_i_sejchas/5924</t>
+  </si>
+  <si>
+    <t>https://t.me/Hvastovichi_segodnya/3867</t>
+  </si>
+  <si>
+    <t>https://t.me/Tvoyo_Ferzikovo/4571</t>
+  </si>
+  <si>
+    <t>https://t.me/Peremyshl_zdes/6734</t>
+  </si>
+  <si>
+    <t>https://t.me/Dela_VMalom/5572</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157230484909473</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_23951</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13219</t>
+  </si>
+  <si>
+    <t>14.07 - 20.07</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13287</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_24088</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157238196137377</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_24090</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157238224383393</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-180268261_61028</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-54813709_752282</t>
+  </si>
+  <si>
+    <t>https://t.me/Dela_VMalom/5587</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-222134246_4255</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000003608141/topic/158032752629069</t>
+  </si>
+  <si>
+    <t>https://ok.ru/raionklg/topic/157399675827161</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-47908301_2792552</t>
+  </si>
+  <si>
+    <t>https://t.me/klgzhest/47063</t>
+  </si>
+  <si>
+    <t>https://t.me/klg_alarm/13281</t>
+  </si>
+  <si>
+    <t>https://vk.com/wall-204895491_24051</t>
+  </si>
+  <si>
+    <t>https://ok.ru/group/70000036196257/topic/157237666082209</t>
   </si>
 </sst>
 </file>
@@ -1907,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,6 +2521,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="26" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2241,9 +2534,288 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14081303-9170-4EFA-93A2-E3A160BF1A11}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>27000</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <f>C2/B2*100</f>
+        <v>0.16296296296296295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3592</v>
+      </c>
+      <c r="C3" s="2">
+        <v>78</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">C3/B3*100</f>
+        <v>2.1714922048997773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2971</v>
+      </c>
+      <c r="C5" s="2">
+        <v>85</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2.8609895658027602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8100</v>
+      </c>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.13580246913580246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" ref="D7" si="1">C7/B7*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="3">
+        <v>114000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.6315789473684209E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="3">
+        <v>81800</v>
+      </c>
+      <c r="C9" s="2">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>8.3129584352078248E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3447</v>
+      </c>
+      <c r="C10" s="2">
+        <v>68</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.9727299100667246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3200</v>
+      </c>
+      <c r="C13">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D19" si="2">C13/B13*100</f>
+        <v>1.65625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B14" s="3">
+        <v>33000</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15" s="3">
+        <v>29900</v>
+      </c>
+      <c r="C15">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.21739130434782608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B17" s="3">
+        <v>76172</v>
+      </c>
+      <c r="C17">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>4.9887097621173132E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B18" s="3">
+        <v>77844</v>
+      </c>
+      <c r="C18">
+        <v>76</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>9.7631159755408245E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3340</v>
+      </c>
+      <c r="C19">
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.6766467065868262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF44B6C-916C-4D23-9E6B-AE95ABFB7419}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
@@ -2268,198 +2840,317 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5">
-        <v>27000</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44</v>
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3">
+        <v>33000</v>
+      </c>
+      <c r="C2">
+        <v>152</v>
       </c>
       <c r="D2">
         <f>C2/B2*100</f>
-        <v>0.16296296296296295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>3592</v>
-      </c>
-      <c r="C3" s="2">
-        <v>78</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D10" si="0">C3/B3*100</f>
-        <v>2.1714922048997773</v>
+        <v>0.46060606060606057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D15" si="0">C3/B3*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3">
+        <v>29800</v>
+      </c>
+      <c r="C4" s="2">
+        <v>135</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.45302013422818793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="3">
+        <v>32600</v>
+      </c>
+      <c r="C5" s="2">
+        <v>127</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.38957055214723929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" ref="D6" si="1">C6/B6*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7">
+        <v>26500</v>
+      </c>
+      <c r="C7">
+        <v>128</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.48301886792452831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9">
+        <v>28300</v>
+      </c>
+      <c r="C9">
+        <v>93</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.32862190812720848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10">
+        <v>29900</v>
+      </c>
+      <c r="C10" s="18">
+        <v>117</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B12" s="2">
+        <v>28400</v>
+      </c>
+      <c r="C12" s="2">
+        <v>68</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.23943661971830987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B14" s="3">
+        <v>29500</v>
+      </c>
+      <c r="C14">
+        <v>178</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.60338983050847461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B15" s="3">
+        <v>29900</v>
+      </c>
+      <c r="C15">
+        <v>291</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.97324414715719065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{0CFF7BCD-B3A2-410D-B795-611949CC8632}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486F4AFC-4924-4E19-95BE-A705AC1FD4BE}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2971</v>
-      </c>
-      <c r="C5" s="2">
-        <v>85</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>2.8609895658027602</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="3">
-        <v>8100</v>
-      </c>
-      <c r="C6" s="2">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.13580246913580246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" ref="D7" si="1">C7/B7*100</f>
-        <v>0</v>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="3">
+        <v>41000</v>
+      </c>
+      <c r="C7">
+        <v>77</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D18" si="0">C7/B7*100</f>
+        <v>0.18780487804878049</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>122</v>
+        <v>469</v>
       </c>
       <c r="B8" s="3">
-        <v>114000</v>
-      </c>
-      <c r="C8" s="2">
-        <v>30</v>
+        <v>7000</v>
+      </c>
+      <c r="C8">
+        <v>57</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>2.6315789473684209E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="3">
-        <v>81800</v>
-      </c>
-      <c r="C9" s="2">
-        <v>68</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>8.3129584352078248E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3447</v>
-      </c>
-      <c r="C10" s="2">
-        <v>68</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.9727299100667246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="B13" s="3">
-        <v>3200</v>
-      </c>
-      <c r="C13">
-        <v>53</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ref="D13:D15" si="2">C13/B13*100</f>
-        <v>1.65625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="B14" s="3">
-        <v>33000</v>
-      </c>
-      <c r="C14">
-        <v>22</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B15" s="3">
-        <v>29900</v>
-      </c>
-      <c r="C15">
-        <v>65</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>0.21739130434782608</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+        <v>0.81428571428571428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>563</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3.4482758620689653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>564</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2468,12 +3159,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF44B6C-916C-4D23-9E6B-AE95ABFB7419}">
-  <dimension ref="A1:D13"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81847137-4DC6-4BE0-AB84-E4D1DABCDF3A}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,287 +3189,6 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="3">
-        <v>33000</v>
-      </c>
-      <c r="C2">
-        <v>152</v>
-      </c>
-      <c r="D2">
-        <f>C2/B2*100</f>
-        <v>0.46060606060606057</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D12" si="0">C3/B3*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="3">
-        <v>29800</v>
-      </c>
-      <c r="C4" s="2">
-        <v>135</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.45302013422818793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="3">
-        <v>32600</v>
-      </c>
-      <c r="C5" s="2">
-        <v>127</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.38957055214723929</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <f t="shared" ref="D6" si="1">C6/B6*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7">
-        <v>26500</v>
-      </c>
-      <c r="C7">
-        <v>128</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.48301886792452831</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>303</v>
-      </c>
-      <c r="B9">
-        <v>28300</v>
-      </c>
-      <c r="C9">
-        <v>93</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.32862190812720848</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>304</v>
-      </c>
-      <c r="B10">
-        <v>29900</v>
-      </c>
-      <c r="C10" s="18">
-        <v>117</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.39130434782608697</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B12" s="2">
-        <v>28400</v>
-      </c>
-      <c r="C12" s="2">
-        <v>68</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.23943661971830987</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{0CFF7BCD-B3A2-410D-B795-611949CC8632}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486F4AFC-4924-4E19-95BE-A705AC1FD4BE}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B7" s="3">
-        <v>41000</v>
-      </c>
-      <c r="C7">
-        <v>77</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D8" si="0">C7/B7*100</f>
-        <v>0.18780487804878049</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B8" s="3">
-        <v>7000</v>
-      </c>
-      <c r="C8">
-        <v>57</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.81428571428571428</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81847137-4DC6-4BE0-AB84-E4D1DABCDF3A}">
-  <dimension ref="A1:D48"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="3">
@@ -3440,6 +3850,176 @@
     <row r="48" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B49" s="3">
+        <v>20887</v>
+      </c>
+      <c r="C49">
+        <v>70</v>
+      </c>
+      <c r="D49" s="15">
+        <f t="shared" ref="D49:D59" si="1">C49/B49*100</f>
+        <v>0.33513668789199025</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1596</v>
+      </c>
+      <c r="C50">
+        <v>72</v>
+      </c>
+      <c r="D50" s="15">
+        <f t="shared" si="1"/>
+        <v>4.5112781954887211</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B51" s="3">
+        <v>16000</v>
+      </c>
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="D51" s="15">
+        <f t="shared" si="1"/>
+        <v>5.6249999999999994E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B52" s="3">
+        <v>143</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" s="15">
+        <f t="shared" si="1"/>
+        <v>2.0979020979020979</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B53" s="3">
+        <v>883</v>
+      </c>
+      <c r="C53">
+        <v>30</v>
+      </c>
+      <c r="D53" s="15">
+        <f t="shared" si="1"/>
+        <v>3.3975084937712339</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B54" s="3">
+        <v>49728</v>
+      </c>
+      <c r="C54">
+        <v>88</v>
+      </c>
+      <c r="D54" s="15">
+        <f t="shared" si="1"/>
+        <v>0.17696267696267698</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B55" s="3">
+        <v>45423</v>
+      </c>
+      <c r="C55">
+        <v>12</v>
+      </c>
+      <c r="D55" s="15">
+        <f t="shared" si="1"/>
+        <v>2.6418334324020867E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B56" s="3">
+        <v>25730</v>
+      </c>
+      <c r="C56">
+        <v>99</v>
+      </c>
+      <c r="D56" s="15">
+        <f t="shared" si="1"/>
+        <v>0.38476486591527403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B57" s="3">
+        <v>16798</v>
+      </c>
+      <c r="C57">
+        <v>73</v>
+      </c>
+      <c r="D57" s="15">
+        <f t="shared" si="1"/>
+        <v>0.43457554470770332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B58" s="3">
+        <v>3121</v>
+      </c>
+      <c r="C58">
+        <v>55</v>
+      </c>
+      <c r="D58" s="15">
+        <f t="shared" si="1"/>
+        <v>1.7622556872797179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B59" s="3">
+        <v>22674</v>
+      </c>
+      <c r="C59">
+        <v>12</v>
+      </c>
+      <c r="D59" s="15">
+        <f t="shared" si="1"/>
+        <v>5.2924053982535059E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -3450,15 +4030,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C59E1B9-CED3-4664-963C-6197669203DC}">
-  <dimension ref="A1:D308"/>
+  <dimension ref="A1:D355"/>
   <sheetViews>
-    <sheetView topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="A308" sqref="A308:XFD308"/>
+    <sheetView topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="H355" sqref="H355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7982,7 +8562,7 @@
         <v>35</v>
       </c>
       <c r="D305">
-        <f t="shared" ref="D305:D307" si="4">C305/B305*100</f>
+        <f t="shared" ref="D305:D358" si="4">C305/B305*100</f>
         <v>3.1687112398714412E-2</v>
       </c>
     </row>
@@ -8019,6 +8599,701 @@
     <row r="308" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A308" s="7" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A309" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B309" s="3">
+        <v>47182</v>
+      </c>
+      <c r="C309">
+        <v>59</v>
+      </c>
+      <c r="D309">
+        <f t="shared" si="4"/>
+        <v>0.12504768767750413</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A310" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B310" s="3">
+        <v>27550</v>
+      </c>
+      <c r="C310">
+        <v>92</v>
+      </c>
+      <c r="D310">
+        <f t="shared" si="4"/>
+        <v>0.33393829401088926</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A311" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B311" s="3">
+        <v>2990</v>
+      </c>
+      <c r="C311">
+        <v>44</v>
+      </c>
+      <c r="D311">
+        <f t="shared" si="4"/>
+        <v>1.471571906354515</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A312" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B312" s="3">
+        <v>9360</v>
+      </c>
+      <c r="C312">
+        <v>561</v>
+      </c>
+      <c r="D312">
+        <f t="shared" si="4"/>
+        <v>5.9935897435897436</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A313" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B313" s="3">
+        <v>17134</v>
+      </c>
+      <c r="C313">
+        <v>17</v>
+      </c>
+      <c r="D313">
+        <f t="shared" si="4"/>
+        <v>9.9217929263452784E-2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A314" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B314" s="3">
+        <v>3220</v>
+      </c>
+      <c r="C314">
+        <v>55</v>
+      </c>
+      <c r="D314">
+        <f t="shared" si="4"/>
+        <v>1.7080745341614907</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A315" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B315" s="3">
+        <v>35642</v>
+      </c>
+      <c r="C315">
+        <v>93</v>
+      </c>
+      <c r="D315">
+        <f t="shared" si="4"/>
+        <v>0.26092811851186803</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A316" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B316" s="3">
+        <v>22263</v>
+      </c>
+      <c r="C316">
+        <v>19</v>
+      </c>
+      <c r="D316">
+        <f t="shared" si="4"/>
+        <v>8.53433948704128E-2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A317" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B317" s="3">
+        <v>44849</v>
+      </c>
+      <c r="C317">
+        <v>93</v>
+      </c>
+      <c r="D317">
+        <f t="shared" si="4"/>
+        <v>0.20736248299850613</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A318" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B318" s="3">
+        <v>3360</v>
+      </c>
+      <c r="C318">
+        <v>59</v>
+      </c>
+      <c r="D318">
+        <f t="shared" si="4"/>
+        <v>1.7559523809523809</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A319" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B319" s="3">
+        <v>15313</v>
+      </c>
+      <c r="C319">
+        <v>142</v>
+      </c>
+      <c r="D319">
+        <f t="shared" si="4"/>
+        <v>0.92731665904786775</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A320" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B320" s="3">
+        <v>49496</v>
+      </c>
+      <c r="C320">
+        <v>87</v>
+      </c>
+      <c r="D320">
+        <f t="shared" si="4"/>
+        <v>0.17577177953774042</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A321" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B321" s="3">
+        <v>44445</v>
+      </c>
+      <c r="C321">
+        <v>30</v>
+      </c>
+      <c r="D321">
+        <f t="shared" si="4"/>
+        <v>6.7499156260546742E-2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A322" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B322" s="3">
+        <v>3350</v>
+      </c>
+      <c r="C322">
+        <v>68</v>
+      </c>
+      <c r="D322">
+        <f t="shared" si="4"/>
+        <v>2.0298507462686568</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A323" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B323" s="3">
+        <v>29633</v>
+      </c>
+      <c r="C323">
+        <v>109</v>
+      </c>
+      <c r="D323">
+        <f t="shared" si="4"/>
+        <v>0.36783315897816621</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A324" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B324" s="3">
+        <v>23685</v>
+      </c>
+      <c r="C324">
+        <v>19</v>
+      </c>
+      <c r="D324">
+        <f t="shared" si="4"/>
+        <v>8.0219548237280974E-2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A325" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B325" s="3">
+        <v>11857</v>
+      </c>
+      <c r="C325">
+        <v>132</v>
+      </c>
+      <c r="D325">
+        <f t="shared" si="4"/>
+        <v>1.1132664248966855</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A326" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="B326" s="3">
+        <v>62203</v>
+      </c>
+      <c r="C326">
+        <v>93</v>
+      </c>
+      <c r="D326">
+        <f t="shared" si="4"/>
+        <v>0.14951047377136151</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A327" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B327" s="3">
+        <v>30500</v>
+      </c>
+      <c r="C327">
+        <v>250</v>
+      </c>
+      <c r="D327">
+        <f t="shared" si="4"/>
+        <v>0.81967213114754101</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A328" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B328" s="3">
+        <v>31100</v>
+      </c>
+      <c r="C328">
+        <v>56</v>
+      </c>
+      <c r="D328">
+        <f t="shared" si="4"/>
+        <v>0.18006430868167203</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A329" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B329" s="3">
+        <v>51998</v>
+      </c>
+      <c r="C329">
+        <v>201</v>
+      </c>
+      <c r="D329">
+        <f t="shared" si="4"/>
+        <v>0.38655332897419131</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A330" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B330" s="3">
+        <v>25049</v>
+      </c>
+      <c r="C330">
+        <v>127</v>
+      </c>
+      <c r="D330">
+        <f t="shared" si="4"/>
+        <v>0.50700626771527801</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A331" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B331" s="3">
+        <v>17144</v>
+      </c>
+      <c r="C331">
+        <v>42</v>
+      </c>
+      <c r="D331">
+        <f t="shared" si="4"/>
+        <v>0.244983667755483</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A332" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B332" s="3">
+        <v>104993</v>
+      </c>
+      <c r="C332">
+        <v>84</v>
+      </c>
+      <c r="D332">
+        <f t="shared" si="4"/>
+        <v>8.0005333688912592E-2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A333" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B333" s="3">
+        <v>2084</v>
+      </c>
+      <c r="C333">
+        <v>28</v>
+      </c>
+      <c r="D333">
+        <f t="shared" si="4"/>
+        <v>1.3435700575815739</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A334" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B334" s="3">
+        <v>12204</v>
+      </c>
+      <c r="C334">
+        <v>47</v>
+      </c>
+      <c r="D334">
+        <f t="shared" si="4"/>
+        <v>0.38511963290724355</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A335" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B335" s="3">
+        <v>69438</v>
+      </c>
+      <c r="C335">
+        <v>230</v>
+      </c>
+      <c r="D335">
+        <f t="shared" si="4"/>
+        <v>0.33123073821250615</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A336" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B336" s="3">
+        <v>267848</v>
+      </c>
+      <c r="C336">
+        <v>49</v>
+      </c>
+      <c r="D336">
+        <f t="shared" si="4"/>
+        <v>1.8293957767091786E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A337" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B337" s="3">
+        <v>119595</v>
+      </c>
+      <c r="C337">
+        <v>103</v>
+      </c>
+      <c r="D337">
+        <f t="shared" si="4"/>
+        <v>8.6124001839541789E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A338" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B338" s="3">
+        <v>66278</v>
+      </c>
+      <c r="C338">
+        <v>84</v>
+      </c>
+      <c r="D338">
+        <f t="shared" si="4"/>
+        <v>0.12673888771538067</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A339" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B339" s="3">
+        <v>3332</v>
+      </c>
+      <c r="C339">
+        <v>100</v>
+      </c>
+      <c r="D339">
+        <f t="shared" si="4"/>
+        <v>3.0012004801920766</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A340" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B340" s="3">
+        <v>3116</v>
+      </c>
+      <c r="C340">
+        <v>42</v>
+      </c>
+      <c r="D340">
+        <f t="shared" si="4"/>
+        <v>1.3478818998716302</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A341" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>560</v>
+      </c>
+      <c r="B342" s="14">
+        <v>634</v>
+      </c>
+      <c r="C342">
+        <v>45</v>
+      </c>
+      <c r="D342">
+        <f t="shared" si="4"/>
+        <v>7.0977917981072558</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>561</v>
+      </c>
+      <c r="B343" s="14">
+        <v>52</v>
+      </c>
+      <c r="C343">
+        <v>1</v>
+      </c>
+      <c r="D343">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769231</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>562</v>
+      </c>
+      <c r="B344" s="14">
+        <v>16</v>
+      </c>
+      <c r="C344">
+        <v>1</v>
+      </c>
+      <c r="D344">
+        <f t="shared" si="4"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>565</v>
+      </c>
+      <c r="B345" s="14">
+        <v>1700</v>
+      </c>
+      <c r="C345">
+        <v>40</v>
+      </c>
+      <c r="D345">
+        <f t="shared" si="4"/>
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>566</v>
+      </c>
+      <c r="B346" s="14">
+        <v>1900</v>
+      </c>
+      <c r="C346">
+        <v>29</v>
+      </c>
+      <c r="D346">
+        <f t="shared" si="4"/>
+        <v>1.5263157894736841</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>567</v>
+      </c>
+      <c r="B347" s="14">
+        <v>200</v>
+      </c>
+      <c r="C347">
+        <v>48</v>
+      </c>
+      <c r="D347">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>568</v>
+      </c>
+      <c r="B348" s="14">
+        <v>6700</v>
+      </c>
+      <c r="C348">
+        <v>23</v>
+      </c>
+      <c r="D348">
+        <f t="shared" si="4"/>
+        <v>0.34328358208955223</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>569</v>
+      </c>
+      <c r="B349" s="14">
+        <v>8700</v>
+      </c>
+      <c r="C349">
+        <v>15</v>
+      </c>
+      <c r="D349">
+        <f t="shared" si="4"/>
+        <v>0.17241379310344829</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>570</v>
+      </c>
+      <c r="B350" s="14">
+        <v>285</v>
+      </c>
+      <c r="C350">
+        <v>10</v>
+      </c>
+      <c r="D350">
+        <f t="shared" si="4"/>
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>571</v>
+      </c>
+      <c r="B351" s="14">
+        <v>7000</v>
+      </c>
+      <c r="C351">
+        <v>67</v>
+      </c>
+      <c r="D351">
+        <f t="shared" si="4"/>
+        <v>0.95714285714285707</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>572</v>
+      </c>
+      <c r="B352" s="14">
+        <v>19200</v>
+      </c>
+      <c r="C352">
+        <v>250</v>
+      </c>
+      <c r="D352">
+        <f t="shared" si="4"/>
+        <v>1.3020833333333335</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>573</v>
+      </c>
+      <c r="B353" s="14">
+        <v>2352</v>
+      </c>
+      <c r="C353">
+        <v>77</v>
+      </c>
+      <c r="D353">
+        <f t="shared" si="4"/>
+        <v>3.2738095238095242</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>574</v>
+      </c>
+      <c r="B354" s="14">
+        <v>20000</v>
+      </c>
+      <c r="C354">
+        <v>86</v>
+      </c>
+      <c r="D354">
+        <f t="shared" si="4"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>575</v>
+      </c>
+      <c r="B355" s="14">
+        <v>8600</v>
+      </c>
+      <c r="C355">
+        <v>22</v>
+      </c>
+      <c r="D355">
+        <f t="shared" si="4"/>
+        <v>0.25581395348837205</v>
       </c>
     </row>
   </sheetData>
@@ -8035,10 +9310,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECD268A-1D1B-4593-9D1D-FD8A45FD1925}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8599,6 +9874,416 @@
         <v>479</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B41" s="3">
+        <v>488</v>
+      </c>
+      <c r="C41">
+        <v>36</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:D67" si="1">C41/B41*100</f>
+        <v>7.3770491803278686</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B42" s="3">
+        <v>955</v>
+      </c>
+      <c r="C42">
+        <v>59</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>6.178010471204189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2230</v>
+      </c>
+      <c r="C43">
+        <v>72</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>3.2286995515695067</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1690</v>
+      </c>
+      <c r="C44">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>3.609467455621302</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1150</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>3.8260869565217388</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2290</v>
+      </c>
+      <c r="C46">
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>1.8777292576419216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B47" s="3">
+        <v>187</v>
+      </c>
+      <c r="C47">
+        <v>35</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>18.71657754010695</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B48" s="3">
+        <v>376</v>
+      </c>
+      <c r="C48">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>9.5744680851063837</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B49" s="3">
+        <v>653</v>
+      </c>
+      <c r="C49">
+        <v>39</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>5.9724349157733538</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B50" s="3">
+        <v>437</v>
+      </c>
+      <c r="C50">
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>9.1533180778032026</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B51" s="3">
+        <v>72</v>
+      </c>
+      <c r="C51">
+        <v>32</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B52" s="3">
+        <v>260</v>
+      </c>
+      <c r="C52">
+        <v>34</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>13.076923076923078</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B53" s="3">
+        <v>374</v>
+      </c>
+      <c r="C53">
+        <v>43</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>11.497326203208557</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B54" s="3">
+        <v>404</v>
+      </c>
+      <c r="C54">
+        <v>36</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>8.9108910891089099</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B55" s="3">
+        <v>506</v>
+      </c>
+      <c r="C55">
+        <v>31</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>6.1264822134387353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B56" s="3">
+        <v>329</v>
+      </c>
+      <c r="C56">
+        <v>39</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>11.854103343465045</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B57" s="3">
+        <v>260</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>15.384615384615385</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B58" s="3">
+        <v>277</v>
+      </c>
+      <c r="C58">
+        <v>33</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>11.913357400722022</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B59" s="3">
+        <v>454</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>6.607929515418502</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B60" s="3">
+        <v>786</v>
+      </c>
+      <c r="C60">
+        <v>56</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>7.1246819338422389</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B61" s="3">
+        <v>399</v>
+      </c>
+      <c r="C61">
+        <v>34</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>8.5213032581453625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B62" s="3">
+        <v>438</v>
+      </c>
+      <c r="C62">
+        <v>35</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>7.9908675799086755</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B63" s="3">
+        <v>383</v>
+      </c>
+      <c r="C63">
+        <v>33</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>8.6161879895561366</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B64" s="3">
+        <v>343</v>
+      </c>
+      <c r="C64">
+        <v>36</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>10.495626822157435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B65" s="3">
+        <v>70339</v>
+      </c>
+      <c r="C65">
+        <v>211</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>0.29997583133112499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B66" s="3">
+        <v>127269</v>
+      </c>
+      <c r="C66">
+        <v>112</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>8.8002577218332823E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B67" s="3">
+        <v>132760</v>
+      </c>
+      <c r="C67">
+        <v>106</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>7.984332630310334E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -8607,10 +10292,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9114231D-599A-42FD-A9FD-84CC03FEAE5E}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8664,7 +10349,7 @@
         <v>103</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D49" si="0">C4/B4*100</f>
+        <f t="shared" ref="D4:D54" si="0">C4/B4*100</f>
         <v>9.1150442477876098E-2</v>
       </c>
     </row>
@@ -9321,18 +11006,86 @@
         <v>479</v>
       </c>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B51" s="3">
+        <v>59533</v>
+      </c>
+      <c r="C51">
+        <v>123</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20660809970940486</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B52" s="3">
+        <v>64318</v>
+      </c>
+      <c r="C52">
+        <v>133</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20678503684816071</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B53" s="3">
+        <v>63799</v>
+      </c>
+      <c r="C53">
+        <v>218</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34169814573896146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>531</v>
+      </c>
+      <c r="B54" s="3">
+        <v>116250</v>
+      </c>
+      <c r="C54">
+        <v>296</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25462365591397851</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A54" r:id="rId1" xr:uid="{6C90B904-099A-47AA-9AC1-3B7B33D68C11}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500971C4-A847-4939-A5E5-85DF2BEEF60A}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9560,6 +11313,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="19" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9568,10 +11326,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726694B7-4482-401C-9FD1-2B06FEEB1E5D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9624,6 +11382,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9632,10 +11395,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F61FF64-7611-43CF-BBDD-E5C45F4E5AE8}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9688,6 +11451,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9696,10 +11464,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A772FBBA-2BCE-4F6F-A598-2C8AFC21352E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9752,6 +11520,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9760,10 +11533,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA696F9-DF40-44FA-A46C-1F218A6DC7C7}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9816,6 +11589,11 @@
         <v>479</v>
       </c>
     </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>